<commit_message>
starting to implement the Transferir functionality
</commit_message>
<xml_diff>
--- a/Data/dados_base.xlsx
+++ b/Data/dados_base.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1410" yWindow="1380" windowWidth="14310" windowHeight="10605" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Saldo" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +26,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,7 +57,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -417,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,10 +449,87 @@
           <t>Desc</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>123/321</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>05/05/2004</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>compras</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>123/321</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>05/05/2004</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>compras</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Saldo</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the Depositar functionality is done
</commit_message>
<xml_diff>
--- a/Data/dados_base.xlsx
+++ b/Data/dados_base.xlsx
@@ -2,15 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1410" yWindow="1380" windowWidth="14310" windowHeight="10605" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Saldo" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,10 +27,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -57,7 +55,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -420,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,41 +451,69 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B2" t="inlineStr">
+        <v>100</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>26/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>56.36</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>26/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>85.90</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>26/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1.58</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>26/02/2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>25.63</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>123/321</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>05/05/2004</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>compras</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>5</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>123/321</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>05/05/2004</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>compras</t>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>26/02/2023</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>cabelo</t>
         </is>
       </c>
     </row>
@@ -502,10 +528,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -524,12 +550,27 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>156.36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>242.26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>243.84</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>218.21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>